<commit_message>
Fix TypeScript unused imports and sync test template files
</commit_message>
<xml_diff>
--- a/client/public/测试集模板.xlsx
+++ b/client/public/测试集模板.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="29000" windowHeight="13620"/>
+    <workbookView windowWidth="29400" windowHeight="14020"/>
   </bookViews>
   <sheets>
     <sheet name="gptbots_evaluation_template_age" sheetId="1" r:id="rId1"/>
@@ -68,16 +68,16 @@
     <t>测量无效的主要原因是什么？怎么解决？ A28：（1）未在肝组织内进行测量。这种情况最常见，操作者可检查屏幕上的超声TM和A模式是否符合质控标准，以确保探头精准定位。 耦合剂不够。操作者可检查是否是耦合剂太少，增加耦合剂。 触碰到肋骨。解决方式同（1） （4）客户病态肥胖。对于超重客户，由于肝脏离皮肤表面太远，使用M探头可能导致无法检测到肝区，提示无效测量。可根据屏幕提示切换大号探头。 （5）客户存在腹水。液体会干扰剪切波的传播，导致测量无效。此种情况需多次切换点位尝试检测，若仍无法检测出有效数值，则需抽取腹水后再进行检测。 （6）客户肋间隙钙化。老年客户肋间隙可能出现钙化，导致测量无效。此种情况需多次切换点位尝试检测，可以请客户身体更加弯曲，以进一步打开肋间隙。</t>
   </si>
   <si>
-    <t>探头校验的必要性和深圳回波校验的唯一性</t>
-  </si>
-  <si>
-    <t>福波看设备是否需要定期维护？---***---是的，探头需要每年校验，确保其性能符合标准，但设备本身不受使用频率影响。</t>
+    <t>探头校验的必要性和深圳xxx校验的唯一性</t>
+  </si>
+  <si>
+    <t>xxx看设备是否需要定期维护？---***---是的，探头需要每年校验，确保其性能符合标准，但设备本身不受使用频率影响。</t>
   </si>
   <si>
     <t>怎么添加操作者账户</t>
   </si>
   <si>
-    <t>20：若护士进行操作，是使用护士账号还是医生的？在报告单上，操作人填写护士还是医生？该操作是否合规？ A20：操作人是谁就登录谁的账号，福波看的操作员无需具备超声资质，医生、护士、技师在接受厂家提供的专业培训，通过考核并获得相应证书后操作检测都是符合规定的。实际操作员是谁，报告单上的操作员就是谁。原则上所有操作员应建立独立的账号，谁操作使用谁的账号，便于客户管理与后续追溯。</t>
+    <t>20：若护士进行操作，是使用护士账号还是医生的？在报告单上，操作人填写护士还是医生？该操作是否合规？ A20：操作人是谁就登录谁的账号，xxx看的操作员无需具备超声资质，医生、护士、技师在接受厂家提供的专业培训，通过考核并获得相应证书后操作检测都是符合规定的。实际操作员是谁，报告单上的操作员就是谁。原则上所有操作员应建立独立的账号，谁操作使用谁的账号，便于客户管理与后续追溯。</t>
   </si>
   <si>
     <t>打印机的清洁</t>
@@ -110,138 +110,138 @@
     <t>探头和设备的日常保养</t>
   </si>
   <si>
-    <t>回波技术原理的优势</t>
-  </si>
-  <si>
-    <t>利用受控振动瞬时弹性成像技术（VCTE），评估肝脏纤维化程度；利用受控衰减参数技术，用于评估肝脏脂肪变程度。 技术原理对比，FibroScan的VCTE技术为同类技术的全球首创。有包括WHO在内的多篇国际指南共识推荐。</t>
-  </si>
-  <si>
-    <t>回波探头的差异</t>
-  </si>
-  <si>
-    <t>回波探头对比原因优势---***---针对常规人群提供7mm直径M+探头, *针对严重超重/肥胖人群提供XL+探头,针对儿童提供S+探头。探头尺寸及针对性适配人群。M+探头经过验证可以适配大部分体检人群。尚无文献佐证单一探头的检查准确性。</t>
-  </si>
-  <si>
-    <t>回波检查定位的优势</t>
-  </si>
-  <si>
-    <t>回波检查定位对比原因优势---***---提供TM超、A超以及US－LTT三重质控定位，实现高效定位肝脏最佳检测位置。可升级新版本：引导式弹性成像技术无需弹性图显示，通过低频连续振动产生剪切波信号，利用剪切波信号进行定位，设备自动判断检测点位是否合格并输出检测数值,降低操作者专业度依赖，提高检测结果可靠性。多重定位实现自动高效准确的检测定位。最大程度减少操作步骤及操作者依赖。同时，无需对超声二维图像进行诊断和判定。 一次检测即可实现肝脏硬度值及肝脏脂肪变程度双参数检测。</t>
-  </si>
-  <si>
-    <t>回波智能深度的优势</t>
-  </si>
-  <si>
-    <t>回波智能深度对比原因优势---***---在不改变探头超声波频率的情况下剪切波探头自动根据探头到肝包膜距离自动调节测量深度。智能深度自动高效准确的检测采样。最大程度减少操作步骤及操作者依赖。</t>
-  </si>
-  <si>
-    <t>回波肝脏脂肪变CAP采集方法的优势</t>
-  </si>
-  <si>
-    <t>回波肝脏脂肪变CAP采集方法对比原因优势---***---a.支持200-5000次CAP连续发射采集，有效降低变异性 b.可选单次CAP采集。 连续CAP可有效降低检测结果的变异性。</t>
-  </si>
-  <si>
-    <t>回波数据质控的优势</t>
-  </si>
-  <si>
-    <t>回波数据质控对比原因优势---***---非肝区或肝脏检测位置不佳会提示无效检测，自动脱落数据。多维质控算法，确保检测结果稳定，准确。</t>
-  </si>
-  <si>
-    <t>回波检查结果准确性的优势</t>
-  </si>
-  <si>
-    <t>回波检查结果准确性对比原因优势---***---肝脏硬度LSM和肝脏脂肪变CAP与肝活检相比，检测结果一致性高达90%以上，临床效能好。全球超过200篇指南明确了FibroScan检测准确性和临床效能。</t>
-  </si>
-  <si>
-    <t>回波界值选择的优势</t>
-  </si>
-  <si>
-    <t>回波界值选择准确性对比原因优势---***---提供有文献依据的，包括健康体检、乙肝、丙肝等多种病因的界值选择。同类TE厂家均参考了VCTE的界值解读。但WHO明确指出：FibroScan®的临界值不适用于其它品牌的瞬时弹性成像技术。</t>
-  </si>
-  <si>
-    <t>回波评分模型</t>
-  </si>
-  <si>
-    <t xml:space="preserve">回波评分模型对比原因优势---***---基于LSM和CAP值，可以使用包括FAST在内的多种评分模型，有效预测包括MASH在内的多种肝病进展风险。 *评分模型已内置在Connect工作站。将FibroScan®检查结果（采用LSM by VCTE™ &amp; CAP™）与易于获取的血液生物标志物（AST）相结合的评分算法，有助于在即时医疗场所识别显著性纤维化MASH患者，减少侵入性及昂贵的检查。
+    <t>xxx技术原理的优势</t>
+  </si>
+  <si>
+    <t>利用受控振动瞬时弹性成像技术（VCTE），评估肝脏纤维化程度；利用受控衰减参数技术，用于评估肝脏脂肪变程度。 技术原理对比，xxxScan的VCTE技术为同类技术的全球首创。有包括WHO在内的多篇国际指南共识推荐。</t>
+  </si>
+  <si>
+    <t>xxx探头的差异</t>
+  </si>
+  <si>
+    <t>xxx探头对比原因优势---***---针对常规人群提供7mm直径M+探头, *针对严重超重/肥胖人群提供XL+探头,针对儿童提供S+探头。探头尺寸及针对性适配人群。M+探头经过验证可以适配大部分体检人群。尚无文献佐证单一探头的检查准确性。</t>
+  </si>
+  <si>
+    <t>xxx检查定位的优势</t>
+  </si>
+  <si>
+    <t>xxx检查定位对比原因优势---***---提供TM超、A超以及US－LTT三重质控定位，实现高效定位肝脏最佳检测位置。可升级新版本：引导式弹性成像技术无需弹性图显示，通过低频连续振动产生剪切波信号，利用剪切波信号进行定位，设备自动判断检测点位是否合格并输出检测数值,降低操作者专业度依赖，提高检测结果可靠性。多重定位实现自动高效准确的检测定位。最大程度减少操作步骤及操作者依赖。同时，无需对超声二维图像进行诊断和判定。 一次检测即可实现肝脏硬度值及肝脏脂肪变程度双参数检测。</t>
+  </si>
+  <si>
+    <t>xxx智能深度的优势</t>
+  </si>
+  <si>
+    <t>xxx智能深度对比原因优势---***---在不改变探头超声波频率的情况下剪切波探头自动根据探头到肝包膜距离自动调节测量深度。智能深度自动高效准确的检测采样。最大程度减少操作步骤及操作者依赖。</t>
+  </si>
+  <si>
+    <t>xxx肝脏脂肪变CAP采集方法的优势</t>
+  </si>
+  <si>
+    <t>xxx肝脏脂肪变CAP采集方法对比原因优势---***---a.支持200-5000次CAP连续发射采集，有效降低变异性 b.可选单次CAP采集。 连续CAP可有效降低检测结果的变异性。</t>
+  </si>
+  <si>
+    <t>xxx数据质控的优势</t>
+  </si>
+  <si>
+    <t>xxx数据质控对比原因优势---***---非肝区或肝脏检测位置不佳会提示无效检测，自动脱落数据。多维质控算法，确保检测结果稳定，准确。</t>
+  </si>
+  <si>
+    <t>xxx检查结果准确性的优势</t>
+  </si>
+  <si>
+    <t>xxx检查结果准确性对比原因优势---***---肝脏硬度LSM和肝脏脂肪变CAP与肝活检相比，检测结果一致性高达90%以上，临床效能好。全球超过200篇指南明确了xxxScan检测准确性和临床效能。</t>
+  </si>
+  <si>
+    <t>xxx界值选择的优势</t>
+  </si>
+  <si>
+    <t>xxx界值选择准确性对比原因优势---***---提供有文献依据的，包括健康体检、乙肝、丙肝等多种病因的界值选择。同类TE厂家均参考了VCTE的界值解读。但WHO明确指出：xxxScan®的临界值不适用于其它品牌的瞬时弹性成像技术。</t>
+  </si>
+  <si>
+    <t>xxx评分模型</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xxx评分模型对比原因优势---***---基于LSM和CAP值，可以使用包括FAST在内的多种评分模型，有效预测包括MASH在内的多种肝病进展风险。 *评分模型已内置在Connect工作站。将xxxScan®检查结果（采用LSM by VCTE™ &amp; CAP™）与易于获取的血液生物标志物（AST）相结合的评分算法，有助于在即时医疗场所识别显著性纤维化MASH患者，减少侵入性及昂贵的检查。
 </t>
   </si>
   <si>
-    <t>回波用药指导及优势</t>
-  </si>
-  <si>
-    <t>回波用药指导对比原因优势---***---多种肝病、内分泌相关药物在临床评价阶段使用FibroScan作为分期管理和用药监测的无创评估手段。经严格验证，FibroScan可用于用药评估、使用监测。</t>
-  </si>
-  <si>
-    <t>回波脾脏硬度检测的优势</t>
-  </si>
-  <si>
-    <t>回波脾脏硬度检测对比原因优势---***---具备有技术研究基础，充分循证的脾脏硬度检测功能。基于VCTE的SSM技术已纳入。已获Baveno VII 共识推荐：SSM≤ 40 kPa可用于识别高危静脉曲张概率低的患者，以豁免胃镜检查。</t>
+    <t>xxx用药指导及优势</t>
+  </si>
+  <si>
+    <t>xxx用药指导对比原因优势---***---多种肝病、内分泌相关药物在临床评价阶段使用xxxScan作为分期管理和用药监测的无创评估手段。经严格验证，xxxScan可用于用药评估、使用监测。</t>
+  </si>
+  <si>
+    <t>xxx脾脏硬度检测的优势</t>
+  </si>
+  <si>
+    <t>xxx脾脏硬度检测对比原因优势---***---具备有技术研究基础，充分循证的脾脏硬度检测功能。基于VCTE的SSM技术已纳入。已获Baveno VII 共识推荐：SSM≤ 40 kPa可用于识别高危静脉曲张概率低的患者，以豁免胃镜检查。</t>
   </si>
   <si>
     <t>甘纤尺 vs VCTE 对比</t>
   </si>
   <si>
-    <t>甘纤尺与VCTE对比 区别---***---肝纤维化：肝细胞组织在持续急慢性炎症状态下被相关炎症因子反复损坏后再生胶原纤维和蛋白多糖等大量细胞外基质(extracellular matrix, ECM)，并在肝脏中过度沉积和异常分布。其中，肝星状细胞(HSC)是肝脏组织中细胞外基质(ECM)的主要来源，当肝脏受到持续严重损害时，HSCs 由相对静止表型向活化表型逐渐转化，进一步获得肌成纤维母细胞(Myofibrolast MFB)的特征是肝纤维化进展过程的核心环节。在肝脏损伤的早期阶段，CHI3L1由肝巨噬细胞释放进一步激活肝星状细胞，反过来，通过自分泌方式产生 CHI3L1蛋白从而形成循环，肝纤维化晚期阶段，激活的肝星状细胞分化成产生 1 型胶原蛋白的肌成纤维细胞，从而导致肝纤维化。</t>
-  </si>
-  <si>
-    <t>福波看与其他肝脏检测设备相比，主要优势有哪些？</t>
-  </si>
-  <si>
-    <t>福波看的优势主要包括：
+    <t>甘纤尺与VCTE对比 区别---***---肝纤维化：肝细胞组织在持续急慢性炎症状态下被相关炎症因子反复损坏后再生胶原纤维和蛋白多糖等大量细胞外基质(extracellular matrix, ECM)，并在肝脏中过度沉积和异常分布。其中，肝星状细胞(HSC)是肝脏组织中细胞外基质(ECM)的主要来源，当肝脏受到持续严重损害时，HSCs 由相对静止表型向活化表型逐渐转化，进一步获得肌成纤维母细胞(Myoxxxlast MFB)的特征是肝纤维化进展过程的核心环节。在肝脏损伤的早期阶段，CHI3L1由肝巨噬细胞释放进一步激活肝星状细胞，反过来，通过自分泌方式产生 CHI3L1蛋白从而形成循环，肝纤维化晚期阶段，激活的肝星状细胞分化成产生 1 型胶原蛋白的肌成纤维细胞，从而导致肝纤维化。</t>
+  </si>
+  <si>
+    <t>xxx看与其他肝脏检测设备相比，主要优势有哪些？</t>
+  </si>
+  <si>
+    <t>xxx看的优势主要包括：
 （1）无创安全，患者接受度高；
 （2）快速精准，3-5分钟出结果，与肝活检一致性＞90%；
 （3）量化检测，支持长期变化监测；
 （4）早期病变一测就知，避免漏诊。</t>
   </si>
   <si>
-    <t>福波看采用的VCTE™技术与普通超声弹性成像有何区别？</t>
-  </si>
-  <si>
-    <t>福波看的VCTE™技术能产生频率固定的剪切波，通过测量其传播速度定量计算肝组织硬度，有专利和明确标准。普通超声弹性成像的剪切波由超声束转化而来，频率不固定，能量有损耗，导致结果差异大且无统一标准。</t>
-  </si>
-  <si>
-    <t>福波看检测前是否需要空腹？为什么？</t>
+    <t>xxx看采用的VCTE™技术与普通超声弹性成像有何区别？</t>
+  </si>
+  <si>
+    <t>xxx看的VCTE™技术能产生频率固定的剪切波，通过测量其传播速度定量计算肝组织硬度，有专利和明确标准。普通超声弹性成像的剪切波由超声束转化而来，频率不固定，能量有损耗，导致结果差异大且无统一标准。</t>
+  </si>
+  <si>
+    <t>xxx看检测前是否需要空腹？为什么？</t>
   </si>
   <si>
     <t>需要。餐后血液动力学改变会导致肝脏硬度值比实际偏高，为保证结果准确，检测前需至少空腹3小时。</t>
   </si>
   <si>
-    <t>福波看检测是否有辐射？孕妇可以使用吗？</t>
+    <t>xxx看检测是否有辐射？孕妇可以使用吗？</t>
   </si>
   <si>
     <t>没有辐射。它采用声波和机械波原理，无电离辐射。2024年美国FDA已明确说明孕妇等特殊人群也可以使用。</t>
   </si>
   <si>
-    <t>福波看检测一次需要多长时间？流程是怎样的？</t>
+    <t>xxx看检测一次需要多长时间？流程是怎样的？</t>
   </si>
   <si>
     <t>全程仅需3-5分钟。具体流程：客户躺下，涂抹耦合剂，用探头在右肋间轻扫（实际扫描2-3分钟），设备自动分析后当场显示肝脏硬度和脂肪含量的数值。</t>
   </si>
   <si>
-    <t>福波看检测是否有年龄限制？儿童可以使用吗？</t>
+    <t>xxx看检测是否有年龄限制？儿童可以使用吗？</t>
   </si>
   <si>
     <t>没有年龄限制。儿童可以使用，选择模式的唯一标准是胸围：胸围≤45cm用S1探头，45cm＜胸围≤75cm用S2探头。甚至有针对婴儿（如胆道闭锁）的应用报道。</t>
   </si>
   <si>
-    <t>饮酒对福波看检测结果有什么影响？饮酒后多久可以检测？</t>
+    <t>饮酒对xxx看检测结果有什么影响？饮酒后多久可以检测？</t>
   </si>
   <si>
     <t>酒精会导致肝脏硬度值高估。建议客户戒酒一周后再进行检测。参考标准：男性饮酒＞30g/天，女性＞20g/天即为大量饮酒。</t>
   </si>
   <si>
-    <t>福波看检测有哪些禁忌症？</t>
+    <t>xxx看检测有哪些禁忌症？</t>
   </si>
   <si>
     <t>无绝对禁忌症，基本适用于所有人群。区别在于结果是否易受影响，如严重肥胖、腹水可能影响结果准确性，但仅存在无效测量的风险，无其他风险。</t>
   </si>
   <si>
-    <t>福波看操作者是否需要具备超声资质？</t>
+    <t>xxx看操作者是否需要具备超声资质？</t>
   </si>
   <si>
     <t>不需要。操作者（医生、护士、技师均可）经过厂家培训（约100次检测）并取得授权证书后即可操作，无须具备超声资质。</t>
   </si>
   <si>
-    <t>如何选择福波看的探头型号？M和XL探头分别适用于哪些人群？</t>
+    <t>如何选择xxx看的探头型号？M和XL探头分别适用于哪些人群？</t>
   </si>
   <si>
     <t>应遵循设备界面推荐。爱康主要铺设M探头（标配），适用于大部分人群。XL探头适用于200斤以上的肥胖或腹型肥胖人群，以确保剪切波有效传播。</t>
@@ -259,7 +259,7 @@
 （6）肋间隙钙化（老年人）：多次换点尝试，让身体更弯曲以打开肋间隙。</t>
   </si>
   <si>
-    <t>福波看的质控标准包括哪些内容？</t>
+    <t>xxx看的质控标准包括哪些内容？</t>
   </si>
   <si>
     <t>通过三重质控：
@@ -268,7 +268,7 @@
 （3）数据校验（同一位置≥10次有效检测，IQR/中值≤30%，CAP进度条≥100%）。</t>
   </si>
   <si>
-    <t>福波看检测结果必须由谁解读？为什么？</t>
+    <t>xxx看检测结果必须由谁解读？为什么？</t>
   </si>
   <si>
     <t>必须由专业医生解读。因为医生需结合患者的完整病历、检查质量（有效次数、IQR等）、以及影响肝脏硬度的潜在因素进行综合诊断，设备结果仅为辅助诊断指标。</t>
@@ -286,23 +286,23 @@
     <t>不一定。E值高提示肝硬化风险，但需结合其他检查综合判断。急性肝炎等也可能暂时拉高数值，需医生排除干扰后再下结论。</t>
   </si>
   <si>
-    <t>转氨酶升高是否会影响福波看的检测结果？</t>
+    <t>转氨酶升高是否会影响xxx看的检测结果？</t>
   </si>
   <si>
     <t>会。肝脏炎症以及AST/ALT显著升高（超过正常值上限5倍）会导致肝脏硬度测量值（E值）假性升高，可能高估肝纤维化程度。建议炎症缓解后重新评估。</t>
   </si>
   <si>
-    <t>福波看检测结果与肝纤四项相比有何优势？</t>
-  </si>
-  <si>
-    <t>福波看直接测量肝脏硬度，无创、快速、准确性高（与肝活检一致性＞90%），能量化分期（F0-F4）并同时检测脂肪肝。肝纤四项为间接提示，易受炎症、肾功能等因素干扰，特异性和准确性较低。</t>
-  </si>
-  <si>
-    <t>福波看与“甘纤尺”、“甘欣安”等检测项目有何区别？</t>
+    <t>xxx看检测结果与肝纤四项相比有何优势？</t>
+  </si>
+  <si>
+    <t>xxx看直接测量肝脏硬度，无创、快速、准确性高（与肝活检一致性＞90%），能量化分期（F0-F4）并同时检测脂肪肝。肝纤四项为间接提示，易受炎症、肾功能等因素干扰，特异性和准确性较低。</t>
+  </si>
+  <si>
+    <t>xxx看与“甘纤尺”、“甘欣安”等检测项目有何区别？</t>
   </si>
   <si>
     <t>主要区别在于：
-福波看：检测LSM和CAP，用于筛查、诊断、疗效监测全流程，无创、可重复、量化，结果即时。
+xxx看：检测LSM和CAP，用于筛查、诊断、疗效监测全流程，无创、可重复、量化，结果即时。
 甘纤尺：检测壳酶蛋白（CHI3L1），用于肝纤维化筛查，需血液检测等待数天，对轻度纤维化诊断价值有限。
 甘欣安：检测cfDNA甲基化，用于肝癌初筛，需血液检测等待数天，是筛查肝癌而非肝纤维化的手段。
 应用场景和临床价值不同，不建议直接对比。</t>
@@ -314,10 +314,10 @@
     <t>首先排除质控不达标和短期影响因素（如是否空腹、心率、饮酒、体位）。若均排除，结果仍高，建议客户3个月、6个月复诊对比随访，或到医院进一步检查。应向客户解释肝硬度受多种因素（饱腹、心率、饮酒等）影响，长期动态对比更有意义。</t>
   </si>
   <si>
-    <t>福波看是否支持外检？有哪些型号支持移动使用？</t>
-  </si>
-  <si>
-    <t>可以外检。分院可走MIS外检流程带设备到客户端服务。福波看HANDY型号设备有两种使用模式：（1）连接电源；（2）使用自带电池，电池可待机5小时，检测使用2小时。具体案例可联系区域对接人员。</t>
+    <t>xxx看是否支持外检？有哪些型号支持移动使用？</t>
+  </si>
+  <si>
+    <t>可以外检。分院可走MIS外检流程带设备到客户端服务。xxx看HANDY型号设备有两种使用模式：（1）连接电源；（2）使用自带电池，电池可待机5小时，检测使用2小时。具体案例可联系区域对接人员。</t>
   </si>
 </sst>
 </file>
@@ -1472,8 +1472,8 @@
   <sheetPr/>
   <dimension ref="A1:B51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleSheetLayoutView="60" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" zoomScaleSheetLayoutView="60" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="M39" sqref="B12 M39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.3846153846154" defaultRowHeight="16.8" outlineLevelCol="1"/>

</xml_diff>